<commit_message>
added team acronyms, distributed side bar to more pages and realigned pages
</commit_message>
<xml_diff>
--- a/Fantasy2024.xlsx
+++ b/Fantasy2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Fantasy Football 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F353A98-47DC-441C-83F2-52AF182CCBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B1106E-3472-4485-807E-BF767CA8EDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{84D6A58F-B445-4F4B-BFDB-8866828E621E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{84D6A58F-B445-4F4B-BFDB-8866828E621E}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15005" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15018" uniqueCount="852">
   <si>
     <t>Category</t>
   </si>
@@ -2564,6 +2564,45 @@
   <si>
     <t>Tutu Atwell</t>
   </si>
+  <si>
+    <t>Acronym</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>MRD</t>
+  </si>
+  <si>
+    <t>OU</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>THAr</t>
+  </si>
+  <si>
+    <t>KDT</t>
+  </si>
+  <si>
+    <t>CNC</t>
+  </si>
+  <si>
+    <t>JG</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>AAT</t>
+  </si>
 </sst>
 </file>
 
@@ -2885,11 +2924,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B5DD735-7CCA-45C5-B3B0-B4C1B2CC6419}" name="TeamsTable" displayName="TeamsTable" ref="A1:D13" totalsRowShown="0">
-  <autoFilter ref="A1:D13" xr:uid="{1B5DD735-7CCA-45C5-B3B0-B4C1B2CC6419}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B5DD735-7CCA-45C5-B3B0-B4C1B2CC6419}" name="TeamsTable" displayName="TeamsTable" ref="A1:E13" totalsRowShown="0">
+  <autoFilter ref="A1:E13" xr:uid="{1B5DD735-7CCA-45C5-B3B0-B4C1B2CC6419}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{39025A10-64F1-4B66-9952-5905F997A9BE}" name="Manager Name"/>
     <tableColumn id="2" xr3:uid="{1EC40674-7C0B-4206-B11F-AA34BF2C38F5}" name="Fantasy Name"/>
+    <tableColumn id="5" xr3:uid="{529E43E0-42D3-4A24-A197-647153107BC9}" name="Acronym"/>
     <tableColumn id="3" xr3:uid="{A77CD583-BACE-4F9C-A375-4D424D0B1CCD}" name="Division"/>
     <tableColumn id="4" xr3:uid="{76DCF35D-E5C3-4704-AA8B-467AF64A12EA}" name="Image"/>
   </tableColumns>
@@ -9141,21 +9181,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD9E349-3DA3-447A-9608-EB048412ACEB}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="102.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="102.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -9163,13 +9204,16 @@
         <v>167</v>
       </c>
       <c r="C1" t="s">
+        <v>839</v>
+      </c>
+      <c r="D1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -9177,13 +9221,16 @@
         <v>120</v>
       </c>
       <c r="C2" t="s">
+        <v>840</v>
+      </c>
+      <c r="D2" t="s">
         <v>124</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -9191,13 +9238,16 @@
         <v>125</v>
       </c>
       <c r="C3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D3" t="s">
         <v>124</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -9205,13 +9255,16 @@
         <v>127</v>
       </c>
       <c r="C4" t="s">
+        <v>842</v>
+      </c>
+      <c r="D4" t="s">
         <v>124</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -9219,13 +9272,16 @@
         <v>129</v>
       </c>
       <c r="C5" t="s">
+        <v>843</v>
+      </c>
+      <c r="D5" t="s">
         <v>124</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -9233,13 +9289,16 @@
         <v>131</v>
       </c>
       <c r="C6" t="s">
+        <v>844</v>
+      </c>
+      <c r="D6" t="s">
         <v>124</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -9247,13 +9306,16 @@
         <v>133</v>
       </c>
       <c r="C7" t="s">
+        <v>845</v>
+      </c>
+      <c r="D7" t="s">
         <v>124</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -9261,13 +9323,16 @@
         <v>137</v>
       </c>
       <c r="C8" t="s">
+        <v>846</v>
+      </c>
+      <c r="D8" t="s">
         <v>135</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -9275,13 +9340,16 @@
         <v>139</v>
       </c>
       <c r="C9" t="s">
+        <v>847</v>
+      </c>
+      <c r="D9" t="s">
         <v>135</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -9289,13 +9357,16 @@
         <v>141</v>
       </c>
       <c r="C10" t="s">
+        <v>848</v>
+      </c>
+      <c r="D10" t="s">
         <v>135</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -9303,13 +9374,16 @@
         <v>143</v>
       </c>
       <c r="C11" t="s">
+        <v>849</v>
+      </c>
+      <c r="D11" t="s">
         <v>135</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -9317,13 +9391,16 @@
         <v>145</v>
       </c>
       <c r="C12" t="s">
+        <v>850</v>
+      </c>
+      <c r="D12" t="s">
         <v>135</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -9331,9 +9408,12 @@
         <v>829</v>
       </c>
       <c r="C13" t="s">
+        <v>851</v>
+      </c>
+      <c r="D13" t="s">
         <v>135</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>823</v>
       </c>
     </row>
@@ -18582,11 +18662,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9039B0B5-3B27-4C71-AC3A-92612F4F2087}">
   <dimension ref="A1:AL1226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D1039" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D1106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1123" sqref="C1123"/>
+      <selection pane="bottomRight" activeCell="G1234" sqref="G1234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added fumble returned for TD stat, not common and wasn't there at start of season. McBride got one
</commit_message>
<xml_diff>
--- a/Fantasy2024.xlsx
+++ b/Fantasy2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Fantasy Football 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C5D50E-9D34-494C-A367-5FAA69E72B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788E8C35-A670-44F0-8A50-2FC859892632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{84D6A58F-B445-4F4B-BFDB-8866828E621E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{84D6A58F-B445-4F4B-BFDB-8866828E621E}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15018" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15021" uniqueCount="854">
   <si>
     <t>Category</t>
   </si>
@@ -2603,6 +2603,12 @@
   <si>
     <t>AAT</t>
   </si>
+  <si>
+    <t>Fumble Recovered for TD</t>
+  </si>
+  <si>
+    <t>FTD</t>
+  </si>
 </sst>
 </file>
 
@@ -2836,8 +2842,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AA39457B-F82D-48CD-8053-2972EEA12CE2}" name="ScoringTable" displayName="ScoringTable" ref="A1:D58" totalsRowShown="0">
-  <autoFilter ref="A1:D58" xr:uid="{AA39457B-F82D-48CD-8053-2972EEA12CE2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AA39457B-F82D-48CD-8053-2972EEA12CE2}" name="ScoringTable" displayName="ScoringTable" ref="A1:D59" totalsRowShown="0">
+  <autoFilter ref="A1:D59" xr:uid="{AA39457B-F82D-48CD-8053-2972EEA12CE2}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{BF7C11C0-F2C3-44BD-89A1-F8704136D88E}" name="Category"/>
     <tableColumn id="2" xr3:uid="{F90B0D90-EA17-406A-9846-3CC2FDC03855}" name="Stat"/>
@@ -3473,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A773FA-4D4B-49BD-97B9-0EF3185FFD79}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4296,6 +4302,20 @@
       </c>
       <c r="D58">
         <v>-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>852</v>
+      </c>
+      <c r="C59" t="s">
+        <v>853</v>
+      </c>
+      <c r="D59">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -18662,7 +18682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9039B0B5-3B27-4C71-AC3A-92612F4F2087}">
   <dimension ref="A1:AL1226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
continued to fix injured and traded/fa players
</commit_message>
<xml_diff>
--- a/Fantasy2024.xlsx
+++ b/Fantasy2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Fantasy Football 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788E8C35-A670-44F0-8A50-2FC859892632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFBF88F-99AB-405E-A0AD-F0CF094EA82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{84D6A58F-B445-4F4B-BFDB-8866828E621E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{84D6A58F-B445-4F4B-BFDB-8866828E621E}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring" sheetId="1" r:id="rId1"/>
@@ -3048,7 +3048,7 @@
   <autoFilter ref="A2:AL1226" xr:uid="{29D8D1DD-6E27-42F4-8EEC-6CB433104867}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Brandon Cooks"/>
+        <filter val="Rico Dawdle"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3481,7 +3481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A773FA-4D4B-49BD-97B9-0EF3185FFD79}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
@@ -18682,11 +18682,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9039B0B5-3B27-4C71-AC3A-92612F4F2087}">
   <dimension ref="A1:AL1226"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G68" sqref="G68"/>
+      <selection pane="bottomRight" activeCell="G1229" sqref="G1229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19181,7 +19181,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -19519,7 +19519,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -19967,7 +19967,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>3</v>
       </c>
@@ -20647,7 +20647,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4</v>
       </c>
@@ -27627,7 +27627,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>1</v>
       </c>
@@ -27635,7 +27635,7 @@
         <v>131</v>
       </c>
       <c r="C324" t="s">
-        <v>336</v>
+        <v>835</v>
       </c>
       <c r="D324" t="s">
         <v>198</v>
@@ -28043,7 +28043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>2</v>
       </c>
@@ -28051,7 +28051,7 @@
         <v>131</v>
       </c>
       <c r="C340" t="s">
-        <v>336</v>
+        <v>835</v>
       </c>
       <c r="D340" t="s">
         <v>198</v>
@@ -28433,7 +28433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>3</v>
       </c>
@@ -28441,7 +28441,7 @@
         <v>131</v>
       </c>
       <c r="C355" t="s">
-        <v>336</v>
+        <v>835</v>
       </c>
       <c r="D355" t="s">
         <v>198</v>
@@ -28875,7 +28875,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="372" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>4</v>
       </c>
@@ -28883,7 +28883,7 @@
         <v>131</v>
       </c>
       <c r="C372" t="s">
-        <v>336</v>
+        <v>835</v>
       </c>
       <c r="D372" t="s">
         <v>198</v>
@@ -29197,7 +29197,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="383" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>5</v>
       </c>
@@ -29205,7 +29205,7 @@
         <v>131</v>
       </c>
       <c r="C383" t="s">
-        <v>336</v>
+        <v>835</v>
       </c>
       <c r="D383" t="s">
         <v>198</v>
@@ -29575,7 +29575,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="395" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>6</v>
       </c>
@@ -29583,7 +29583,7 @@
         <v>131</v>
       </c>
       <c r="C395" t="s">
-        <v>336</v>
+        <v>835</v>
       </c>
       <c r="D395" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
separated R code for nfl team data, cleaned out real names, added abbrev names for draft, fixed draft board page and used abbre names for spacing
</commit_message>
<xml_diff>
--- a/Fantasy2024.xlsx
+++ b/Fantasy2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Fantasy Football 24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFBF88F-99AB-405E-A0AD-F0CF094EA82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61772AF-FE3A-40D2-B973-73A7D4789C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{84D6A58F-B445-4F4B-BFDB-8866828E621E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{84D6A58F-B445-4F4B-BFDB-8866828E621E}"/>
   </bookViews>
   <sheets>
     <sheet name="Scoring" sheetId="1" r:id="rId1"/>
@@ -2945,16 +2945,7 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C1D0A848-22A7-46E7-91A0-0415A3EB3E7F}" name="NFLteamsTable" displayName="NFLteamsTable" ref="A1:O36" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:O36" xr:uid="{C1D0A848-22A7-46E7-91A0-0415A3EB3E7F}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Atlanta Falcons"/>
-        <filter val="Dallas Cowboys"/>
-        <filter val="New Orleans Saints"/>
-        <filter val="Pittsburgh Steelers"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O36" xr:uid="{C1D0A848-22A7-46E7-91A0-0415A3EB3E7F}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{EF28E491-171D-4FA6-AF8A-E06CF75A8FF4}" name="team_abbr"/>
     <tableColumn id="2" xr3:uid="{B50CA952-43AB-4433-B283-3D7DA82143D1}" name="team_name"/>
@@ -9450,7 +9441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D875B8-A97C-420A-8881-14670F8DB865}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
@@ -9518,7 +9509,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>267</v>
       </c>
@@ -9612,7 +9603,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>246</v>
       </c>
@@ -9659,7 +9650,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>202</v>
       </c>
@@ -9706,7 +9697,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>190</v>
       </c>
@@ -9753,7 +9744,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>192</v>
       </c>
@@ -9800,7 +9791,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>248</v>
       </c>
@@ -9847,7 +9838,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -9941,7 +9932,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>209</v>
       </c>
@@ -9988,7 +9979,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>282</v>
       </c>
@@ -10035,7 +10026,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>148</v>
       </c>
@@ -10082,7 +10073,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>200</v>
       </c>
@@ -10129,7 +10120,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>250</v>
       </c>
@@ -10176,7 +10167,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>255</v>
       </c>
@@ -10223,7 +10214,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>252</v>
       </c>
@@ -10270,7 +10261,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>638</v>
       </c>
@@ -10317,7 +10308,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>256</v>
       </c>
@@ -10364,7 +10355,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -10411,7 +10402,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>207</v>
       </c>
@@ -10458,7 +10449,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>232</v>
       </c>
@@ -10505,7 +10496,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>213</v>
       </c>
@@ -10552,7 +10543,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>230</v>
       </c>
@@ -10646,7 +10637,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>261</v>
       </c>
@@ -10693,7 +10684,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>217</v>
       </c>
@@ -10734,7 +10725,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>706</v>
       </c>
@@ -10781,7 +10772,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>225</v>
       </c>
@@ -10875,7 +10866,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>721</v>
       </c>
@@ -10922,7 +10913,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>264</v>
       </c>
@@ -10969,7 +10960,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -11016,7 +11007,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>239</v>
       </c>
@@ -11063,7 +11054,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>262</v>
       </c>
@@ -11110,7 +11101,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>750</v>
       </c>
@@ -18682,7 +18673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9039B0B5-3B27-4C71-AC3A-92612F4F2087}">
   <dimension ref="A1:AL1226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>